<commit_message>
Sixth Commit encapsulating driver class in every class pages
</commit_message>
<xml_diff>
--- a/FreeCRMTest/Testdata/SpreadSheetData.xlsx
+++ b/FreeCRMTest/Testdata/SpreadSheetData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="4">
   <si>
     <t>Result</t>
   </si>
@@ -368,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -388,7 +388,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>